<commit_message>
Revert "Merge branch 'main' of https://github.com/cfetch1/Senior-Design"
This reverts commit 6cadba857d326a241c8084622f44d31b0b287cba, reversing
changes made to 797e567a643a87844e2012652ec24b225d401915.
</commit_message>
<xml_diff>
--- a/New Folder/Drag.xlsx
+++ b/New Folder/Drag.xlsx
@@ -418,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10924">
+  <borders count="9996">
     <border>
       <left/>
       <right/>
@@ -10507,939 +10507,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10953">
+  <cellXfs count="10025">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -21471,934 +20543,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9993" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9994" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9995" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9996" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9997" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9998" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9999" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10000" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10001" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10002" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10003" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10004" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10005" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10006" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10007" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10008" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10009" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10010" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10011" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10012" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10013" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10014" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10015" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10016" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10017" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10018" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10019" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10020" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10021" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10022" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10023" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10024" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10025" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10026" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10027" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10028" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10029" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10030" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10031" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10032" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10033" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10034" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10035" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10036" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10037" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10038" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10039" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10040" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10041" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10042" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10043" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10044" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10045" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10046" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10047" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10048" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10049" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10050" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10051" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10052" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10053" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10054" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10055" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10056" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10057" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10058" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10059" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10060" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10061" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10062" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10063" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10064" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10065" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10066" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10067" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10068" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10069" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10070" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10071" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10072" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10073" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10074" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10075" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10076" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10077" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10078" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10079" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10080" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10081" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10082" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10083" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10084" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10085" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10086" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10087" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10088" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10089" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10090" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10091" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10092" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10093" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10094" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10095" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10096" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10097" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10098" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10099" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10100" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10101" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10102" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10103" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10104" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10105" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10106" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10107" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10108" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10109" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10110" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10111" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10112" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10113" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10114" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10115" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10116" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10117" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10118" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10119" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10120" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10121" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10122" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10123" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10124" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10125" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10126" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10127" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10128" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10129" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10130" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10131" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10132" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10133" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10134" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10135" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10136" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10137" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10138" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10139" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10140" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10141" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10142" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10143" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10144" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10145" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10146" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10147" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10148" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10149" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10150" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10151" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10152" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10153" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10154" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10155" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10156" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10157" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10158" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10159" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10160" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10161" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10162" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10163" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10164" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10165" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10166" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10167" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10168" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10169" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10170" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10171" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10172" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10173" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10174" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10175" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10176" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10177" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10178" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10179" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10180" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10181" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10182" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10183" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10184" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10185" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10186" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10187" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10188" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10189" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10190" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10191" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10192" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10193" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10194" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10195" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10196" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10197" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10198" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10199" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10200" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10201" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10202" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10203" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10204" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10205" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10206" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10207" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10208" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10209" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10210" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10211" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10212" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10213" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10214" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10215" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10216" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10217" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10218" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10219" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10220" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10221" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10222" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10223" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10224" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10225" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10226" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10227" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10228" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10229" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10230" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10231" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10232" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10233" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10234" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10235" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10236" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10237" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10238" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10239" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10240" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10241" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10242" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10243" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10244" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10245" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10246" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10247" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10248" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10249" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10250" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10251" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10252" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10253" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10254" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10255" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10256" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10257" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10258" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10259" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10260" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10261" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10262" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10263" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10264" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10265" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10266" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10267" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10268" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10269" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10270" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10271" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10272" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10273" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10274" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10275" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10276" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10277" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10278" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10279" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10280" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10281" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10282" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10283" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10284" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10285" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10286" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10287" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10288" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10289" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10290" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10291" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10292" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10293" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10294" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10295" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10296" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10297" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10298" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10299" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10300" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10301" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10302" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10303" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10304" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10305" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10306" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10307" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10308" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10309" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10310" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10311" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10312" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10313" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10314" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10315" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10316" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10317" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10318" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10319" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10320" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10321" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10322" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10323" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10324" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10325" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10326" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10327" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10328" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10329" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10330" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10331" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10332" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10333" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10334" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10335" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10336" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10337" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10338" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10339" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10340" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10341" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10342" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10343" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10344" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10345" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10346" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10347" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10348" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10349" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10350" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10351" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10352" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10353" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10354" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10355" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10356" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10357" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10358" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10359" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10360" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10361" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10362" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10363" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10364" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10365" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10366" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10367" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10368" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10369" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10370" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10371" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10372" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10373" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10374" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10375" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10376" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10377" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10378" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10379" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10380" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10381" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10382" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10383" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10384" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10385" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10386" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10387" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10388" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10389" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10390" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10391" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10392" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10393" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10394" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10395" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10396" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10397" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10398" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10399" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10400" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10401" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10402" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10403" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10404" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10405" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10406" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10407" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10408" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10409" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10410" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10411" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10412" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10413" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10414" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10415" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10416" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10417" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10418" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10419" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10420" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10421" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10422" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10423" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10424" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10425" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10426" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10427" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10428" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10429" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10430" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10431" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10432" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10433" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10434" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10435" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10436" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10437" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10438" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10439" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10440" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10441" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10442" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10443" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10444" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10445" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10446" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10447" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10448" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10449" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10450" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10451" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10452" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10453" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10454" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10455" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10456" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10457" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10458" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10459" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10460" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10461" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10462" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10463" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10464" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10465" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10466" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10467" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10468" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10469" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10470" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10471" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10472" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10473" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10474" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10475" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10476" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10477" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10478" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10479" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10480" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10481" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10482" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10483" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10484" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10485" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10486" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10487" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10488" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10489" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10490" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10491" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10492" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10493" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10494" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10495" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10496" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10497" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10498" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10499" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10500" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10501" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10502" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10503" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10504" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10505" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10506" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10507" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10508" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10509" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10510" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10511" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10512" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10513" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10514" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10515" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10516" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10517" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10518" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10519" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10520" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10521" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10522" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10523" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10524" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10525" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10526" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10527" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10528" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10529" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10530" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10531" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10532" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10533" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10534" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10535" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10536" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10537" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10538" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10539" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10540" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10541" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10542" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10543" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10544" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10545" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10546" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10547" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10548" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10549" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10550" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10551" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10552" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10553" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10554" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10555" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10556" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10557" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10558" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10559" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10560" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10561" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10562" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10563" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10564" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10565" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10566" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10567" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10568" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10569" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10570" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10571" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10572" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10573" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10574" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10575" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10576" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10577" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10578" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10579" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10580" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10581" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10582" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10583" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10584" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10585" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10586" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10587" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10588" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10589" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10590" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10591" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10592" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10593" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10594" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10595" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10596" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10597" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10598" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10599" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10600" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10601" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10602" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10603" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10604" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10605" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10606" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10607" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10608" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10609" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10610" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10611" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10612" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10613" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10614" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10615" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10616" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10617" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10618" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10619" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10620" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10621" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10622" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10623" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10624" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10625" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10626" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10627" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10628" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10629" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10630" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10631" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10632" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10633" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10634" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10635" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10636" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10637" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10638" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10639" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10640" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10641" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10642" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10643" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10644" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10645" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10646" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10647" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10648" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10649" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10650" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10651" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10652" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10653" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10654" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10655" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10656" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10657" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10658" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10659" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10660" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10661" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10662" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10663" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10664" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10665" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10666" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10667" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10668" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10669" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10670" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10671" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10672" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10673" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10674" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10675" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10676" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10677" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10678" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10679" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10680" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10681" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10682" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10683" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10684" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10685" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10686" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10687" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10688" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10689" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10690" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10691" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10692" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10693" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10694" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10695" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10696" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10697" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10698" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10699" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10700" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10701" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10702" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10703" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10704" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10705" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10706" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10707" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10708" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10709" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10710" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10711" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10712" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10713" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10714" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10715" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10716" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10717" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10718" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10719" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10720" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10721" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10722" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10723" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10724" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10725" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10726" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10727" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10728" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10729" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10730" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10731" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10732" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10733" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10734" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10735" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10736" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10737" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10738" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10739" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10740" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10741" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10742" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10743" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10744" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10745" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10746" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10747" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10748" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10749" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10750" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10751" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10752" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10753" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10754" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10755" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10756" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10757" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10758" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10759" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10760" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10761" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10762" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10763" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10764" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10765" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10766" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10767" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10768" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10769" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10770" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10771" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10772" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10773" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10774" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10775" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10776" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10777" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10778" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10779" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10780" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10781" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10782" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10783" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10784" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10785" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10786" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10787" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10788" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10789" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10790" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10791" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10792" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10793" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10794" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10795" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10796" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10797" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10798" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10799" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10800" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10801" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10802" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10803" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10804" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10805" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10806" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10807" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10808" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10809" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10810" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10811" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10812" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10813" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10814" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10815" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10816" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10817" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10818" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10819" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10820" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10821" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10822" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10823" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10824" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10825" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10826" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10827" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10828" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10829" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10830" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10831" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10832" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10833" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10834" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10835" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10836" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10837" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10838" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10839" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10840" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10841" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10842" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10843" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10844" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10845" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10846" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10847" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10848" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10849" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10850" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10851" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10852" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10853" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10854" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10855" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10856" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10857" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10858" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10859" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10860" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10861" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10862" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10863" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10864" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10865" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10866" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10867" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10868" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10869" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10870" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10871" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10872" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10873" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10874" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10875" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10876" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10877" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10878" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10879" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10880" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10881" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10882" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10883" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10884" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10885" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10886" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10887" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10888" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10889" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10890" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10891" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10892" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10893" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10894" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10895" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10896" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10897" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10898" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10899" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10900" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10901" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10902" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10903" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10904" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10905" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10906" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10907" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10908" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10909" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10910" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10911" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10912" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10913" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10914" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10915" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10916" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10917" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10918" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10919" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10920" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10921" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10922" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10923" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -25547,7 +23691,7 @@
     <col min="3" max="3" width="10.5546875" bestFit="true" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" bestFit="true" customWidth="true"/>
     <col min="5" max="9" width="10.5546875" bestFit="true" customWidth="true"/>
-    <col min="10" max="10" width="12.7109375" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="13.7109375" bestFit="true" customWidth="true"/>
     <col min="11" max="22" width="10.5546875" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
@@ -25696,7 +23840,7 @@
         <v>13</v>
       </c>
       <c r="J5" s="32">
-        <v>1.7179207238840504</v>
+        <v>1.6873505439715872</v>
       </c>
       <c r="K5" s="36" t="s">
         <v>10</v>
@@ -25729,7 +23873,7 @@
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="27">
-        <v>947.20489485406256</v>
+        <v>923.05285991323319</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>8</v>
@@ -25740,7 +23884,7 @@
         <v>14</v>
       </c>
       <c r="J6" s="32">
-        <v>25.76881085826076</v>
+        <v>25.310258159573806</v>
       </c>
       <c r="K6" s="36" t="s">
         <v>10</v>
@@ -25771,7 +23915,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="7">
-        <v>1.145280482589367</v>
+        <v>1.1249003626477247</v>
       </c>
       <c r="K7" s="37" t="s">
         <v>10</v>
@@ -25923,7 +24067,7 @@
         <v>0.1026</v>
       </c>
       <c r="J14" s="7">
-        <v>0.19633379701532006</v>
+        <v>0.19284006216818142</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="8"/>
@@ -25946,7 +24090,7 @@
         <v>2.8163</v>
       </c>
       <c r="J15" s="7">
-        <v>0.042987596497285188</v>
+        <v>0.04337525741615661</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="8"/>

</xml_diff>